<commit_message>
First working version of split_excel_stats
</commit_message>
<xml_diff>
--- a/+fmri/+test/test.xlsx
+++ b/+fmri/+test/test.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -411,7 +411,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -572,9 +572,6 @@
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>

</xml_diff>